<commit_message>
Narrowed model list to 4 models
</commit_message>
<xml_diff>
--- a/student_intervention/Experiment_results.xlsx
+++ b/student_intervention/Experiment_results.xlsx
@@ -105,7 +105,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +124,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -169,6 +175,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +459,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,22 +758,22 @@
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="7">
         <v>100</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="7">
         <v>1.8200000000000001E-2</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="7">
         <v>0.99219999999999997</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="7">
         <v>0.72799999999999998</v>
       </c>
       <c r="H18" t="s">
@@ -774,42 +781,42 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="7">
         <v>200</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="7">
         <v>1.6400000000000001E-2</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="7">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="7">
         <v>0.99419999999999997</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="7">
         <v>0.74760000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="7">
         <v>300</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="7">
         <v>1.7100000000000001E-2</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="7">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="7">
         <v>0.99390000000000001</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="7">
         <v>0.76300000000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Answered all questions and implemented all code
</commit_message>
<xml_diff>
--- a/student_intervention/Experiment_results.xlsx
+++ b/student_intervention/Experiment_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="12520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="12523"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +154,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -176,6 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,22 +466,22 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.69140625" customWidth="1"/>
+    <col min="2" max="2" width="14.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.15234375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -497,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -520,7 +527,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -540,7 +547,7 @@
         <v>0.72440000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -560,7 +567,7 @@
         <v>0.76339999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -583,7 +590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -603,7 +610,7 @@
         <v>0.70399999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -623,70 +630,70 @@
         <v>0.61019999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="8">
         <v>100</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>1.6E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>0.80559999999999998</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="8">
         <v>0.76500000000000001</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="8">
         <v>200</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
         <v>1.44E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>0.84250000000000003</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="8">
         <v>0.78039999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="8">
         <v>300</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>0.84230000000000005</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="8">
         <v>0.78200000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -709,7 +716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -729,7 +736,7 @@
         <v>0.80649999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -749,7 +756,7 @@
         <v>0.74809999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -757,7 +764,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
@@ -780,7 +787,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>11</v>
       </c>
@@ -800,7 +807,7 @@
         <v>0.74760000000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
@@ -820,7 +827,7 @@
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -843,7 +850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -863,7 +870,7 @@
         <v>0.75590000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -883,7 +890,7 @@
         <v>0.74809999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="6" t="s">
         <v>12</v>
       </c>
@@ -906,7 +913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="6" t="s">
         <v>12</v>
       </c>
@@ -926,7 +933,7 @@
         <v>0.74129999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="6" t="s">
         <v>12</v>
       </c>
@@ -946,7 +953,7 @@
         <v>0.73129999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>13</v>
       </c>
@@ -972,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>13</v>
       </c>
@@ -995,7 +1002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>0.71260000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1038,7 +1045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
@@ -1058,7 +1065,7 @@
         <v>0.78149999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1085,7 @@
         <v>0.78380000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
@@ -1092,16 +1099,16 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="E38" s="2">
-        <v>0.91039999999999999</v>
+        <v>0.85929999999999995</v>
       </c>
       <c r="F38" s="2">
-        <v>0.7087</v>
+        <v>0.76470000000000005</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>15</v>
       </c>
@@ -1109,19 +1116,19 @@
         <v>200</v>
       </c>
       <c r="C39" s="2">
-        <v>5.1999999999999998E-3</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="D39" s="2">
-        <v>4.0000000000000002E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="E39" s="2">
-        <v>0.84209999999999996</v>
+        <v>0.85619999999999996</v>
       </c>
       <c r="F39" s="2">
-        <v>0.7883</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.79139999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
@@ -1129,16 +1136,16 @@
         <v>300</v>
       </c>
       <c r="C40" s="2">
-        <v>3.7000000000000002E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="D40" s="2">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="E40" s="2">
-        <v>0.84350000000000003</v>
+        <v>0.8468</v>
       </c>
       <c r="F40" s="2">
-        <v>0.78200000000000003</v>
+        <v>0.80600000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>